<commit_message>
:boom: V1: deck.gl ARCHIVED
</commit_message>
<xml_diff>
--- a/data/sheets/门店位置坐标点——for 南川.xlsx
+++ b/data/sheets/门店位置坐标点——for 南川.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/projects/ella/map-visualization/data/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B659AEE2-FF85-5F4F-A7CA-DB6E4AE89A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1300E523-6C87-454D-AA39-D13BA6A24D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,7 +1779,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2137,15 +2137,15 @@
       </c>
       <c r="E2">
         <f ca="1">RAND()*100</f>
-        <v>23.142373725269959</v>
+        <v>30.126553162792646</v>
       </c>
       <c r="F2">
         <f ca="1">100+RAND()*100</f>
-        <v>107.74278130146922</v>
+        <v>122.21075569984586</v>
       </c>
       <c r="G2">
         <f ca="1">RAND()*10000</f>
-        <v>709.61337445221147</v>
+        <v>675.55696879120444</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2163,15 +2163,15 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" ca="1" si="0">RAND()*100</f>
-        <v>4.4709440284963708</v>
+        <v>80.768730756155719</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F66" ca="1" si="1">100+RAND()*100</f>
-        <v>114.60202547344991</v>
+        <v>124.39006199968208</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" ca="1" si="2">RAND()*10000</f>
-        <v>4357.5422150285012</v>
+        <v>8470.134389994615</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2189,15 +2189,15 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>59.042548961857335</v>
+        <v>55.02740159812258</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>198.01906861910703</v>
+        <v>186.70070152424529</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>1013.5609690853242</v>
+        <v>9629.8124379595374</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2215,15 +2215,15 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9384150260918247</v>
+        <v>25.551442239450818</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>110.45913693851321</v>
+        <v>163.8197997493736</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>2169.6949841243418</v>
+        <v>8697.6977580137154</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2241,15 +2241,15 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>90.959445998044671</v>
+        <v>13.471773178697077</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>185.75376580922864</v>
+        <v>139.22026148589418</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>3770.5323531181421</v>
+        <v>8327.944699312</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2267,15 +2267,15 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>78.889774085660733</v>
+        <v>72.617781957967736</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>132.45652709229705</v>
+        <v>109.23624831725095</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>6023.5513926533849</v>
+        <v>422.82293345886177</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2293,15 +2293,15 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>63.145476817375524</v>
+        <v>16.943019411288084</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>130.66553779182908</v>
+        <v>148.15673678511263</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>9991.618419542654</v>
+        <v>5311.037927502367</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2319,15 +2319,15 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>82.187428513897913</v>
+        <v>46.65311376755735</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>180.80751558839631</v>
+        <v>186.59989599895349</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>1369.8614434069057</v>
+        <v>1001.480413372825</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2345,15 +2345,15 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>53.860557004287401</v>
+        <v>5.5759302979965231</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>153.65603766205746</v>
+        <v>191.31010508959815</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>1004.6439933425455</v>
+        <v>266.53857463450612</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2371,15 +2371,15 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>86.866704363885276</v>
+        <v>90.870418602336471</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>123.94874911354569</v>
+        <v>150.8274845724963</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>858.15020893858059</v>
+        <v>7755.4158353207295</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2397,15 +2397,15 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4888583303056677</v>
+        <v>99.364926788603498</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>146.32727874747209</v>
+        <v>151.63666683909094</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>3676.0380674286862</v>
+        <v>295.57441349038152</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2423,15 +2423,15 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>39.933463449456077</v>
+        <v>0.47338058204686728</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>166.7089020617679</v>
+        <v>186.53698765026289</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>1380.0899198444438</v>
+        <v>2979.1560019035469</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2449,15 +2449,15 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>37.865639584454613</v>
+        <v>78.068531932139948</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>195.35480895223924</v>
+        <v>140.85376773610909</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>8065.8332571243527</v>
+        <v>4914.0228762228408</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2475,15 +2475,15 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>59.740182110907149</v>
+        <v>1.2276554630636038</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>179.89759547759957</v>
+        <v>131.49485751186756</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>1360.0077493402607</v>
+        <v>3022.1282865362455</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2501,15 +2501,15 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>85.243984866846233</v>
+        <v>10.878894374777982</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>159.5095145570204</v>
+        <v>119.47230308269782</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>4731.7094938554028</v>
+        <v>1786.8412471248218</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2527,15 +2527,15 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2611712152414993</v>
+        <v>58.518201486414434</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>172.38421600835244</v>
+        <v>120.35062478803113</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>8708.0564088485407</v>
+        <v>4414.7545466006659</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2553,15 +2553,15 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>14.162977810423627</v>
+        <v>85.857712437042323</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>154.64321389428417</v>
+        <v>124.04943218075097</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>8888.603059944031</v>
+        <v>5707.8734647614183</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2579,15 +2579,15 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>59.317858492948375</v>
+        <v>43.983997543278299</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>134.37645165905056</v>
+        <v>155.69694674738986</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
-        <v>1932.789798331107</v>
+        <v>3648.2464382395897</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2605,15 +2605,15 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>61.902033248040254</v>
+        <v>29.855068543215037</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>193.69856138591661</v>
+        <v>155.12981170742245</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>1083.7343101410013</v>
+        <v>2186.9377912202294</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2631,15 +2631,15 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>32.920359108476262</v>
+        <v>3.499264845530814</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>176.59696787196523</v>
+        <v>118.42088673105243</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>9765.550111873863</v>
+        <v>2564.1732683977416</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2657,15 +2657,15 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>40.88716384360044</v>
+        <v>73.16686823953323</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>124.43790405994505</v>
+        <v>104.10002898967245</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>8734.5845489395124</v>
+        <v>3692.7559912309262</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2683,15 +2683,15 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>93.623382213526895</v>
+        <v>48.467543507017567</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>152.72669046649804</v>
+        <v>127.48509531217668</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>3135.3879706008902</v>
+        <v>2850.5236720861117</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2709,15 +2709,15 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>64.680921942985975</v>
+        <v>52.309661591253864</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>190.40643278348807</v>
+        <v>118.71704796876942</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>8221.5772208598628</v>
+        <v>8014.1183265280588</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2735,15 +2735,15 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>37.496678712572617</v>
+        <v>35.108210262675499</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>118.43439341896801</v>
+        <v>152.99036858555147</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>3485.6748566929518</v>
+        <v>2837.4401712174345</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2761,15 +2761,15 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>31.59072866540399</v>
+        <v>97.865406910933189</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>130.31332275129876</v>
+        <v>133.63329417089807</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>3092.6753812353904</v>
+        <v>8626.7503711445297</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2787,15 +2787,15 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>89.761328826988759</v>
+        <v>8.1093134083788492</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>114.22416296627372</v>
+        <v>148.33153292252422</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>3860.5483853615542</v>
+        <v>9586.0573797722645</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2813,15 +2813,15 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>30.995846215038181</v>
+        <v>15.64296143310524</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>109.39523746501187</v>
+        <v>161.39149910232459</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>3120.9150125289452</v>
+        <v>4461.3475744676707</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2839,15 +2839,15 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>53.640204141043434</v>
+        <v>63.442876005875092</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>123.97110824018769</v>
+        <v>177.69612923874166</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>9937.1253788453359</v>
+        <v>6833.7480748952721</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2865,15 +2865,15 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>71.118426111355589</v>
+        <v>98.534448490576963</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>119.02624868241884</v>
+        <v>158.02155954528828</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>1813.9868916197831</v>
+        <v>5438.6025289242471</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2891,15 +2891,15 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8889506272002219</v>
+        <v>20.575267245217876</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>102.40941499291289</v>
+        <v>133.61163209790277</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>8276.2915419303354</v>
+        <v>2027.5004905019832</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2917,15 +2917,15 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5044663865006385</v>
+        <v>84.687359726557233</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
-        <v>153.30189583095392</v>
+        <v>104.95961595204463</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>2614.1957881688681</v>
+        <v>4269.4480781609955</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2943,15 +2943,15 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>30.993994087494535</v>
+        <v>80.902649826106398</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="1"/>
-        <v>120.3076959833612</v>
+        <v>131.28536757445477</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="2"/>
-        <v>6331.3147283344033</v>
+        <v>7866.0091253402934</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2969,15 +2969,15 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>75.168700077493597</v>
+        <v>56.466947554409231</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>156.26983023576284</v>
+        <v>189.49704167808906</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="2"/>
-        <v>8507.1648702448238</v>
+        <v>6516.6331898910748</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2995,15 +2995,15 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>27.866861882581329</v>
+        <v>45.360237194184968</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>140.18967644357602</v>
+        <v>134.64925011340966</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="2"/>
-        <v>406.20663260051867</v>
+        <v>3831.4331783445809</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3021,15 +3021,15 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>59.284964801906867</v>
+        <v>91.846055535604293</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>108.76267194366204</v>
+        <v>108.21801597614251</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="2"/>
-        <v>5939.704329337018</v>
+        <v>75.173569971733741</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3047,15 +3047,15 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>85.705811441489161</v>
+        <v>63.810327855045067</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
-        <v>158.07636675127793</v>
+        <v>115.63893305200457</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="2"/>
-        <v>888.62843846585827</v>
+        <v>7789.9904076288794</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3073,15 +3073,15 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>77.315228247794479</v>
+        <v>83.182284169947039</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>185.56363019299516</v>
+        <v>169.45558925184889</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="2"/>
-        <v>6593.0830689842069</v>
+        <v>7033.4254557512268</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3099,15 +3099,15 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>22.638818552414531</v>
+        <v>4.6766832372541867</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>101.02171216918343</v>
+        <v>186.93960064001192</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="2"/>
-        <v>5510.2310238230011</v>
+        <v>2332.4482853804184</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3125,15 +3125,15 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>55.423135965815362</v>
+        <v>31.199532750216207</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
-        <v>117.62359587952122</v>
+        <v>172.37500425950026</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="2"/>
-        <v>663.6847682860581</v>
+        <v>3717.9522754880136</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3151,15 +3151,15 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6835087393211179</v>
+        <v>70.374681561618175</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>103.64797524730736</v>
+        <v>192.41653300419725</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="2"/>
-        <v>9495.73021222645</v>
+        <v>3768.6578349208999</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3177,15 +3177,15 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>63.346386432663039</v>
+        <v>39.722293946134712</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>126.75579738710302</v>
+        <v>123.48783414956605</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="2"/>
-        <v>2380.6023145237764</v>
+        <v>2430.5113346710327</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3203,15 +3203,15 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>37.099384735609689</v>
+        <v>71.380723736290648</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="1"/>
-        <v>148.48605423458298</v>
+        <v>154.7374113807293</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="2"/>
-        <v>9369.4881012837577</v>
+        <v>7474.0468898790787</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3229,15 +3229,15 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>81.159497319043112</v>
+        <v>46.246036640258836</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="1"/>
-        <v>134.80406124086295</v>
+        <v>160.52960286108552</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="2"/>
-        <v>2247.9603177284034</v>
+        <v>604.62766780638663</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3255,15 +3255,15 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="0"/>
-        <v>48.31858614877369</v>
+        <v>88.17032629737011</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="1"/>
-        <v>129.28684191159604</v>
+        <v>112.01635744145494</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="2"/>
-        <v>8681.7342624238918</v>
+        <v>2979.7497225098168</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3281,15 +3281,15 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="0"/>
-        <v>39.216159179651157</v>
+        <v>83.353623556587365</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="1"/>
-        <v>159.21445251232507</v>
+        <v>155.10843035373881</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="2"/>
-        <v>9985.1901882663733</v>
+        <v>9174.1920930332617</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3307,15 +3307,15 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="0"/>
-        <v>53.02967569333503</v>
+        <v>5.3568933849134526</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="1"/>
-        <v>112.56637363534917</v>
+        <v>158.88530211428474</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="2"/>
-        <v>300.44649650329382</v>
+        <v>2265.0965199714501</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3333,15 +3333,15 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="0"/>
-        <v>37.798835013534124</v>
+        <v>91.706972290799285</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="1"/>
-        <v>123.65441521377439</v>
+        <v>191.88590271234028</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="2"/>
-        <v>7348.7740826514946</v>
+        <v>28.014850306030681</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3359,15 +3359,15 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="0"/>
-        <v>83.663295999428286</v>
+        <v>36.263655971200393</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>156.22085593424288</v>
+        <v>107.28479945365507</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="2"/>
-        <v>5255.3575276369693</v>
+        <v>2414.6633762408464</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3385,15 +3385,15 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="0"/>
-        <v>45.352134455512541</v>
+        <v>48.8320427705399</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>111.52297341307167</v>
+        <v>139.42068473206143</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="2"/>
-        <v>1880.362363305461</v>
+        <v>5624.5634172427235</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3411,15 +3411,15 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="0"/>
-        <v>57.702720508181812</v>
+        <v>75.999594998764252</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="1"/>
-        <v>164.47288098446052</v>
+        <v>143.82660953176793</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="2"/>
-        <v>5738.7292138510711</v>
+        <v>1399.9848781854473</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3437,15 +3437,15 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="0"/>
-        <v>17.017480525530114</v>
+        <v>18.115694184791352</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="1"/>
-        <v>148.70891564921465</v>
+        <v>198.24637502156446</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="2"/>
-        <v>4852.960121413972</v>
+        <v>7691.1065817626777</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3463,15 +3463,15 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="0"/>
-        <v>79.745801988700435</v>
+        <v>22.605579912491535</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="1"/>
-        <v>130.97714242975565</v>
+        <v>160.95944002086605</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="2"/>
-        <v>788.00626599437203</v>
+        <v>6837.0385207487507</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3489,15 +3489,15 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="0"/>
-        <v>18.651599814819665</v>
+        <v>24.78018032228675</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="1"/>
-        <v>137.01240501699991</v>
+        <v>103.62816586170379</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="2"/>
-        <v>7732.6016494888627</v>
+        <v>7631.0979923223395</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3515,15 +3515,15 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="0"/>
-        <v>78.599444570388599</v>
+        <v>29.445785159523709</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="1"/>
-        <v>134.48820000909657</v>
+        <v>114.91722106964868</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="2"/>
-        <v>6736.3237211849082</v>
+        <v>8470.3887503173937</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3541,15 +3541,15 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="0"/>
-        <v>21.8431597953889</v>
+        <v>88.687418058882557</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="1"/>
-        <v>199.50792935683177</v>
+        <v>121.58586522503956</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="2"/>
-        <v>9277.9266752428885</v>
+        <v>8094.0791416903712</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3567,15 +3567,15 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="0"/>
-        <v>13.027930556161882</v>
+        <v>32.232273588896923</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="1"/>
-        <v>132.05276239969439</v>
+        <v>104.5296299909896</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="2"/>
-        <v>4836.1717954257147</v>
+        <v>1998.3409114337057</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3593,15 +3593,15 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="0"/>
-        <v>59.555934392898401</v>
+        <v>29.573610099012125</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>123.0007861951787</v>
+        <v>156.59947247933837</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="2"/>
-        <v>6755.0774085802032</v>
+        <v>7067.5115306593561</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3619,15 +3619,15 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="0"/>
-        <v>14.875766852373696</v>
+        <v>78.356642410198035</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="1"/>
-        <v>109.82671758746054</v>
+        <v>107.57734757033595</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="2"/>
-        <v>9498.9766315758297</v>
+        <v>6249.4084586937333</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3645,15 +3645,15 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="0"/>
-        <v>70.655762505094941</v>
+        <v>55.251024546912156</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="1"/>
-        <v>138.39585130219896</v>
+        <v>155.26590361479657</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="2"/>
-        <v>9425.736786536967</v>
+        <v>8675.0090584447535</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3671,15 +3671,15 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="0"/>
-        <v>27.925797513430783</v>
+        <v>49.272181311583786</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="1"/>
-        <v>124.00878685769798</v>
+        <v>194.66318928331043</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="2"/>
-        <v>7064.8126787404071</v>
+        <v>4853.5622915405984</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3697,15 +3697,15 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="0"/>
-        <v>50.625611192976748</v>
+        <v>71.434853417601104</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="1"/>
-        <v>181.32921666632799</v>
+        <v>138.62282326030476</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="2"/>
-        <v>3108.8928748873914</v>
+        <v>2416.2563566633821</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3723,15 +3723,15 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="0"/>
-        <v>26.445083517377011</v>
+        <v>90.694432545028448</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="1"/>
-        <v>170.04651060193177</v>
+        <v>164.41729637339211</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="2"/>
-        <v>488.94893368722325</v>
+        <v>6409.745336718117</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3749,15 +3749,15 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="0"/>
-        <v>3.035633171047647</v>
+        <v>76.589155801017213</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="1"/>
-        <v>100.59779183045919</v>
+        <v>168.84587287286763</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="2"/>
-        <v>2750.3378432418858</v>
+        <v>5066.0079611731417</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3775,15 +3775,15 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="0"/>
-        <v>97.065710477237658</v>
+        <v>33.909357792229422</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="1"/>
-        <v>165.13171330739172</v>
+        <v>132.18107160937217</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="2"/>
-        <v>784.87689794026755</v>
+        <v>5791.5181857519437</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3801,15 +3801,15 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="0"/>
-        <v>45.321353513750054</v>
+        <v>91.93118553178418</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="1"/>
-        <v>154.54119593515171</v>
+        <v>167.33039941786888</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="2"/>
-        <v>9243.220665111874</v>
+        <v>695.56360545457221</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3827,15 +3827,15 @@
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E130" ca="1" si="3">RAND()*100</f>
-        <v>82.061409734857591</v>
+        <v>93.730983777891424</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F130" ca="1" si="4">100+RAND()*100</f>
-        <v>134.46910493674562</v>
+        <v>122.38616895464695</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G130" ca="1" si="5">RAND()*10000</f>
-        <v>7719.0774427358147</v>
+        <v>7953.7608609442204</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3853,15 +3853,15 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9581450605234307</v>
+        <v>57.70042762646117</v>
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="4"/>
-        <v>148.82416003486978</v>
+        <v>103.2085239652644</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="5"/>
-        <v>1986.1250987048284</v>
+        <v>1621.777042992092</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3879,15 +3879,15 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="3"/>
-        <v>56.827247342574694</v>
+        <v>54.864725012942415</v>
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="4"/>
-        <v>139.1765889443856</v>
+        <v>138.72359335908916</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="5"/>
-        <v>904.95229547812528</v>
+        <v>5227.6706735581165</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3905,15 +3905,15 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="3"/>
-        <v>91.498868775275071</v>
+        <v>4.0834247532759216</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="4"/>
-        <v>188.76257623038936</v>
+        <v>183.88732065383962</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="5"/>
-        <v>302.54320510331723</v>
+        <v>1879.7146108906104</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3931,15 +3931,15 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="3"/>
-        <v>36.673457444412136</v>
+        <v>30.78946506453012</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="4"/>
-        <v>174.64052159948534</v>
+        <v>169.42289149418338</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="5"/>
-        <v>3325.8303556990068</v>
+        <v>4334.2792239560877</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3957,15 +3957,15 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="3"/>
-        <v>71.80123644972744</v>
+        <v>94.197079346930437</v>
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="4"/>
-        <v>103.44663081944344</v>
+        <v>196.14466365112361</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="5"/>
-        <v>1005.5949026308908</v>
+        <v>3463.8376576240848</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3983,15 +3983,15 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="3"/>
-        <v>87.016922042897548</v>
+        <v>88.667279628007506</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="4"/>
-        <v>177.47226209889692</v>
+        <v>135.64043792119332</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="5"/>
-        <v>8340.3456967783513</v>
+        <v>5075.326649509052</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -4009,15 +4009,15 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="3"/>
-        <v>78.843605692747985</v>
+        <v>96.358559254309313</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="4"/>
-        <v>106.7907358505629</v>
+        <v>148.29664330853649</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="5"/>
-        <v>1418.1705024556368</v>
+        <v>6690.9036295696687</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -4035,15 +4035,15 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="3"/>
-        <v>40.034790380969078</v>
+        <v>69.199347861228119</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="4"/>
-        <v>146.30730621466518</v>
+        <v>181.65572641624607</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="5"/>
-        <v>6733.926466810748</v>
+        <v>297.78674055867759</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -4061,15 +4061,15 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="3"/>
-        <v>45.965622710007011</v>
+        <v>71.109562551533912</v>
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="4"/>
-        <v>171.6507814796841</v>
+        <v>115.89461248425302</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="5"/>
-        <v>4562.3430627827865</v>
+        <v>4122.7899641308168</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -4087,15 +4087,15 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="3"/>
-        <v>9.2729439179822357</v>
+        <v>26.323438408909517</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="4"/>
-        <v>176.43105012272497</v>
+        <v>156.97363357188902</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="5"/>
-        <v>4877.0567897214005</v>
+        <v>330.88244200535132</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -4113,15 +4113,15 @@
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="3"/>
-        <v>72.822330499319122</v>
+        <v>88.084587755183179</v>
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="4"/>
-        <v>167.65526532307308</v>
+        <v>138.00093834591195</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="5"/>
-        <v>9930.8225690190538</v>
+        <v>9813.7099789048625</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -4139,15 +4139,15 @@
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7269132264888754</v>
+        <v>4.4714494000563825</v>
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="4"/>
-        <v>144.59267843212004</v>
+        <v>171.78862534708259</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="5"/>
-        <v>2238.9697873763748</v>
+        <v>2000.2153462107574</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4165,15 +4165,15 @@
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="3"/>
-        <v>78.696936566502856</v>
+        <v>63.11294570164069</v>
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="4"/>
-        <v>106.74267747861315</v>
+        <v>125.96633565562129</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="5"/>
-        <v>6303.119123696677</v>
+        <v>2011.9899998300684</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4191,15 +4191,15 @@
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="3"/>
-        <v>61.624835055670104</v>
+        <v>97.772910356401539</v>
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="4"/>
-        <v>121.81491493006656</v>
+        <v>170.50908541541409</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="5"/>
-        <v>4475.3929015139229</v>
+        <v>3361.4406559185295</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4217,15 +4217,15 @@
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="3"/>
-        <v>8.834015508421766</v>
+        <v>11.194134138767087</v>
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="4"/>
-        <v>164.09352684566738</v>
+        <v>179.19263702494266</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="5"/>
-        <v>9484.7968767356197</v>
+        <v>159.68464550031425</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4243,15 +4243,15 @@
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="3"/>
-        <v>45.036700778344098</v>
+        <v>6.4851438742844936</v>
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="4"/>
-        <v>108.8047644549018</v>
+        <v>172.83270309652218</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="5"/>
-        <v>9579.0687459724413</v>
+        <v>1865.7359386469918</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4269,15 +4269,15 @@
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="3"/>
-        <v>76.383420452648764</v>
+        <v>40.727818306781252</v>
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="4"/>
-        <v>181.03566007699891</v>
+        <v>102.61478479611525</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="5"/>
-        <v>8726.3294954735775</v>
+        <v>9778.6672228274492</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4295,15 +4295,15 @@
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="3"/>
-        <v>19.489940888084746</v>
+        <v>45.759152143660373</v>
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="4"/>
-        <v>125.58461724134806</v>
+        <v>162.8437597223535</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="5"/>
-        <v>7555.5175132803706</v>
+        <v>3679.6293575639593</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4321,15 +4321,15 @@
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="3"/>
-        <v>42.846493328791922</v>
+        <v>40.979161474029148</v>
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="4"/>
-        <v>188.12471874531838</v>
+        <v>178.11363497846946</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="5"/>
-        <v>6949.7267555070275</v>
+        <v>6626.4198449053592</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4347,15 +4347,15 @@
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="3"/>
-        <v>88.943227663871852</v>
+        <v>25.644729312744865</v>
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="4"/>
-        <v>173.00352136609328</v>
+        <v>158.2967005965647</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="5"/>
-        <v>3991.8667019148202</v>
+        <v>402.72294819404755</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4373,15 +4373,15 @@
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="3"/>
-        <v>98.385947846225804</v>
+        <v>68.108690056241755</v>
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="4"/>
-        <v>193.95435757913285</v>
+        <v>144.08658775193919</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="5"/>
-        <v>6472.8551271512224</v>
+        <v>1212.2036120322666</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4399,15 +4399,15 @@
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="3"/>
-        <v>77.954571099773645</v>
+        <v>14.827976255674846</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="4"/>
-        <v>172.83762136295476</v>
+        <v>183.29556490172308</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="5"/>
-        <v>1064.1003204692502</v>
+        <v>4594.7805188788707</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4425,15 +4425,15 @@
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="3"/>
-        <v>70.62046673043038</v>
+        <v>23.641624276913255</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="4"/>
-        <v>111.79722382165581</v>
+        <v>173.99376989878786</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="5"/>
-        <v>5866.4113718776316</v>
+        <v>8584.8663190357092</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4451,15 +4451,15 @@
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="3"/>
-        <v>59.048342869623859</v>
+        <v>96.746767288165969</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="4"/>
-        <v>144.68883626256786</v>
+        <v>182.88182813235608</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="5"/>
-        <v>4476.240843006206</v>
+        <v>9331.7569985302416</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4477,15 +4477,15 @@
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="3"/>
-        <v>20.428881110292153</v>
+        <v>26.427166126060776</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="4"/>
-        <v>190.17861244056593</v>
+        <v>176.97628477142558</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="5"/>
-        <v>5250.754116709878</v>
+        <v>1231.0717601508481</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4503,15 +4503,15 @@
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="3"/>
-        <v>53.453639809757789</v>
+        <v>85.739226564121523</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="4"/>
-        <v>126.10141024649138</v>
+        <v>108.91396260806418</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="5"/>
-        <v>4628.0927720970885</v>
+        <v>2345.2114794890522</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4529,15 +4529,15 @@
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="3"/>
-        <v>40.554885908165261</v>
+        <v>69.838972462819854</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="4"/>
-        <v>102.91718818620217</v>
+        <v>190.93278791001467</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="5"/>
-        <v>1561.2024617436982</v>
+        <v>9905.9653119094801</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4555,15 +4555,15 @@
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="3"/>
-        <v>98.019243872915013</v>
+        <v>53.997913654448816</v>
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="4"/>
-        <v>137.774044321698</v>
+        <v>136.15782321892931</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="5"/>
-        <v>6650.1998120433345</v>
+        <v>3541.0161317250399</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4581,15 +4581,15 @@
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="3"/>
-        <v>53.382439183552158</v>
+        <v>34.026298789950502</v>
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="4"/>
-        <v>103.4864890474387</v>
+        <v>161.53830590694827</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="5"/>
-        <v>5916.9905328193663</v>
+        <v>4679.3120453584943</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -4607,15 +4607,15 @@
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="3"/>
-        <v>14.056363823357598</v>
+        <v>11.026796007115713</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="4"/>
-        <v>114.73331313566271</v>
+        <v>109.33436329422129</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="5"/>
-        <v>6166.1393969640967</v>
+        <v>9189.3225501069483</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -4633,15 +4633,15 @@
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="3"/>
-        <v>61.174336960372813</v>
+        <v>33.345374339089275</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="4"/>
-        <v>112.61527840873526</v>
+        <v>185.78327454739383</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="5"/>
-        <v>8399.5867790539887</v>
+        <v>6782.3677537163494</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -4659,15 +4659,15 @@
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="3"/>
-        <v>52.231291962500904</v>
+        <v>73.330945930979041</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="4"/>
-        <v>103.00855862223625</v>
+        <v>103.44980971980372</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="5"/>
-        <v>2172.2345202373949</v>
+        <v>7502.8216128238791</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -4685,15 +4685,15 @@
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="3"/>
-        <v>66.363179305419578</v>
+        <v>73.563934599669793</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="4"/>
-        <v>112.37404129690273</v>
+        <v>102.1838223687889</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="5"/>
-        <v>6189.0063285534034</v>
+        <v>870.3043777924313</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -4711,15 +4711,15 @@
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="3"/>
-        <v>78.450976608644226</v>
+        <v>59.604273442407631</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="4"/>
-        <v>134.26298502674052</v>
+        <v>148.16256857068367</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="5"/>
-        <v>7928.2214858254783</v>
+        <v>3523.6448230668261</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -4737,15 +4737,15 @@
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="3"/>
-        <v>18.635808494161843</v>
+        <v>74.181018905734248</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="4"/>
-        <v>179.97116309336377</v>
+        <v>194.65409337263665</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="5"/>
-        <v>2715.1556849599988</v>
+        <v>7884.8070154829738</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4763,15 +4763,15 @@
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="3"/>
-        <v>93.023147683661065</v>
+        <v>85.455022673806852</v>
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="4"/>
-        <v>136.20513884092298</v>
+        <v>108.3987484864931</v>
       </c>
       <c r="G103">
         <f t="shared" ca="1" si="5"/>
-        <v>4740.38356797905</v>
+        <v>816.22793626649479</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -4789,15 +4789,15 @@
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="3"/>
-        <v>85.40031434258853</v>
+        <v>88.194373873930758</v>
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="4"/>
-        <v>199.59503773972173</v>
+        <v>140.83209260938281</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="5"/>
-        <v>8775.8960738270325</v>
+        <v>6473.6952554116297</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4815,15 +4815,15 @@
       </c>
       <c r="E105">
         <f t="shared" ca="1" si="3"/>
-        <v>90.223009346050958</v>
+        <v>91.965185484575713</v>
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="4"/>
-        <v>174.83469056805609</v>
+        <v>173.43671275765638</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="5"/>
-        <v>4090.5522833401342</v>
+        <v>8264.3678871338125</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4841,15 +4841,15 @@
       </c>
       <c r="E106">
         <f t="shared" ca="1" si="3"/>
-        <v>76.091620591962155</v>
+        <v>97.452265811703768</v>
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="4"/>
-        <v>111.15970422147205</v>
+        <v>192.27569098831236</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="5"/>
-        <v>8026.6276883473074</v>
+        <v>9564.8236487811082</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -4867,15 +4867,15 @@
       </c>
       <c r="E107">
         <f t="shared" ca="1" si="3"/>
-        <v>66.545989435778708</v>
+        <v>87.72636632904036</v>
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="4"/>
-        <v>171.56926124383162</v>
+        <v>120.33647551417999</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="5"/>
-        <v>2016.9476243202289</v>
+        <v>3409.8660223812403</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4893,15 +4893,15 @@
       </c>
       <c r="E108">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67032648689658858</v>
+        <v>48.440941805904934</v>
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="4"/>
-        <v>145.71188585194022</v>
+        <v>139.36755291912573</v>
       </c>
       <c r="G108">
         <f t="shared" ca="1" si="5"/>
-        <v>9055.9326807074849</v>
+        <v>5379.6765340462962</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4919,15 +4919,15 @@
       </c>
       <c r="E109">
         <f t="shared" ca="1" si="3"/>
-        <v>69.61772160730186</v>
+        <v>69.708573186939887</v>
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="4"/>
-        <v>166.97783327151654</v>
+        <v>194.66254136749495</v>
       </c>
       <c r="G109">
         <f t="shared" ca="1" si="5"/>
-        <v>1244.9345068552952</v>
+        <v>299.58657747912287</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -4945,15 +4945,15 @@
       </c>
       <c r="E110">
         <f t="shared" ca="1" si="3"/>
-        <v>74.38340872363699</v>
+        <v>96.396626006523618</v>
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="4"/>
-        <v>168.07350863033889</v>
+        <v>170.20934598570517</v>
       </c>
       <c r="G110">
         <f t="shared" ca="1" si="5"/>
-        <v>8713.8100033424435</v>
+        <v>8930.9944707192608</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4971,15 +4971,15 @@
       </c>
       <c r="E111">
         <f t="shared" ca="1" si="3"/>
-        <v>69.384631742706631</v>
+        <v>0.43807602373764354</v>
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="4"/>
-        <v>177.5591667375175</v>
+        <v>192.59144360960215</v>
       </c>
       <c r="G111">
         <f t="shared" ca="1" si="5"/>
-        <v>2723.1496273072999</v>
+        <v>2062.9721988431306</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4997,15 +4997,15 @@
       </c>
       <c r="E112">
         <f t="shared" ca="1" si="3"/>
-        <v>83.549830648636473</v>
+        <v>84.47800599840869</v>
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="4"/>
-        <v>169.71644488264451</v>
+        <v>184.19741295687754</v>
       </c>
       <c r="G112">
         <f t="shared" ca="1" si="5"/>
-        <v>3827.8425527404634</v>
+        <v>3028.720887424281</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -5023,15 +5023,15 @@
       </c>
       <c r="E113">
         <f t="shared" ca="1" si="3"/>
-        <v>13.848635236362272</v>
+        <v>7.06213886501118</v>
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="4"/>
-        <v>112.33249373779425</v>
+        <v>130.86938259824217</v>
       </c>
       <c r="G113">
         <f t="shared" ca="1" si="5"/>
-        <v>9133.720992459941</v>
+        <v>8998.893398758235</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -5049,15 +5049,15 @@
       </c>
       <c r="E114">
         <f t="shared" ca="1" si="3"/>
-        <v>18.896545716341638</v>
+        <v>14.117526445308826</v>
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="4"/>
-        <v>198.19372661243108</v>
+        <v>155.69499802663137</v>
       </c>
       <c r="G114">
         <f t="shared" ca="1" si="5"/>
-        <v>8799.0464642736861</v>
+        <v>7817.5391489434305</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -5075,15 +5075,15 @@
       </c>
       <c r="E115">
         <f t="shared" ca="1" si="3"/>
-        <v>27.029114794017271</v>
+        <v>82.923423965100639</v>
       </c>
       <c r="F115">
         <f t="shared" ca="1" si="4"/>
-        <v>199.1352515758382</v>
+        <v>125.72778747869644</v>
       </c>
       <c r="G115">
         <f t="shared" ca="1" si="5"/>
-        <v>6360.067543834346</v>
+        <v>5477.5741744704246</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -5101,15 +5101,15 @@
       </c>
       <c r="E116">
         <f t="shared" ca="1" si="3"/>
-        <v>68.934803391155825</v>
+        <v>23.039499224725791</v>
       </c>
       <c r="F116">
         <f t="shared" ca="1" si="4"/>
-        <v>162.01504529420455</v>
+        <v>193.83514195843321</v>
       </c>
       <c r="G116">
         <f t="shared" ca="1" si="5"/>
-        <v>8949.0190232139157</v>
+        <v>3735.8672990516038</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -5127,15 +5127,15 @@
       </c>
       <c r="E117">
         <f t="shared" ca="1" si="3"/>
-        <v>52.658104215030342</v>
+        <v>74.760928135091007</v>
       </c>
       <c r="F117">
         <f t="shared" ca="1" si="4"/>
-        <v>118.16714314890552</v>
+        <v>156.7440539784659</v>
       </c>
       <c r="G117">
         <f t="shared" ca="1" si="5"/>
-        <v>1411.0188525944545</v>
+        <v>4255.5494812810621</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -5153,15 +5153,15 @@
       </c>
       <c r="E118">
         <f t="shared" ca="1" si="3"/>
-        <v>39.15343584631772</v>
+        <v>77.272882305924554</v>
       </c>
       <c r="F118">
         <f t="shared" ca="1" si="4"/>
-        <v>138.70486304783751</v>
+        <v>166.19656516423231</v>
       </c>
       <c r="G118">
         <f t="shared" ca="1" si="5"/>
-        <v>7529.5829203104058</v>
+        <v>322.47688585669397</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -5179,15 +5179,15 @@
       </c>
       <c r="E119">
         <f t="shared" ca="1" si="3"/>
-        <v>14.08936948649937</v>
+        <v>4.5474448750705943</v>
       </c>
       <c r="F119">
         <f t="shared" ca="1" si="4"/>
-        <v>106.34167554118901</v>
+        <v>107.44000656482083</v>
       </c>
       <c r="G119">
         <f t="shared" ca="1" si="5"/>
-        <v>3822.9466548402556</v>
+        <v>6543.0167443421014</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -5205,15 +5205,15 @@
       </c>
       <c r="E120">
         <f t="shared" ca="1" si="3"/>
-        <v>30.111901812591501</v>
+        <v>14.067450366207424</v>
       </c>
       <c r="F120">
         <f t="shared" ca="1" si="4"/>
-        <v>191.18173108032997</v>
+        <v>194.43461396267756</v>
       </c>
       <c r="G120">
         <f t="shared" ca="1" si="5"/>
-        <v>146.03182599254416</v>
+        <v>5124.963323512934</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -5231,15 +5231,15 @@
       </c>
       <c r="E121">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3113651248339742</v>
+        <v>58.708379560140742</v>
       </c>
       <c r="F121">
         <f t="shared" ca="1" si="4"/>
-        <v>106.70550834622284</v>
+        <v>126.79152437870806</v>
       </c>
       <c r="G121">
         <f t="shared" ca="1" si="5"/>
-        <v>5684.642032470987</v>
+        <v>8786.0313620819725</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -5257,15 +5257,15 @@
       </c>
       <c r="E122">
         <f t="shared" ca="1" si="3"/>
-        <v>98.988895751809352</v>
+        <v>91.110044405735877</v>
       </c>
       <c r="F122">
         <f t="shared" ca="1" si="4"/>
-        <v>125.70973374384758</v>
+        <v>111.4182696161387</v>
       </c>
       <c r="G122">
         <f t="shared" ca="1" si="5"/>
-        <v>9735.93568553562</v>
+        <v>2839.216807934376</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -5283,15 +5283,15 @@
       </c>
       <c r="E123">
         <f t="shared" ca="1" si="3"/>
-        <v>83.815853741383123</v>
+        <v>12.726459953669966</v>
       </c>
       <c r="F123">
         <f t="shared" ca="1" si="4"/>
-        <v>162.25559752387448</v>
+        <v>113.88223787615206</v>
       </c>
       <c r="G123">
         <f t="shared" ca="1" si="5"/>
-        <v>3455.0031317598141</v>
+        <v>6271.2567616877577</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -5309,15 +5309,15 @@
       </c>
       <c r="E124">
         <f t="shared" ca="1" si="3"/>
-        <v>12.997378716695085</v>
+        <v>92.62374759723609</v>
       </c>
       <c r="F124">
         <f t="shared" ca="1" si="4"/>
-        <v>185.70850548107347</v>
+        <v>120.20605914565778</v>
       </c>
       <c r="G124">
         <f t="shared" ca="1" si="5"/>
-        <v>6071.0156745705326</v>
+        <v>5494.4862759703228</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -5335,15 +5335,15 @@
       </c>
       <c r="E125">
         <f t="shared" ca="1" si="3"/>
-        <v>4.814476334574036</v>
+        <v>45.761905857217947</v>
       </c>
       <c r="F125">
         <f t="shared" ca="1" si="4"/>
-        <v>132.98079020864293</v>
+        <v>163.01126200519039</v>
       </c>
       <c r="G125">
         <f t="shared" ca="1" si="5"/>
-        <v>6816.7168426730514</v>
+        <v>7983.323532478802</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -5361,15 +5361,15 @@
       </c>
       <c r="E126">
         <f t="shared" ca="1" si="3"/>
-        <v>91.167581635205096</v>
+        <v>25.145674423713103</v>
       </c>
       <c r="F126">
         <f t="shared" ca="1" si="4"/>
-        <v>132.20135836666208</v>
+        <v>183.95804948608475</v>
       </c>
       <c r="G126">
         <f t="shared" ca="1" si="5"/>
-        <v>7451.7853011530524</v>
+        <v>6937.4275907820338</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -5387,15 +5387,15 @@
       </c>
       <c r="E127">
         <f t="shared" ca="1" si="3"/>
-        <v>91.498519904484851</v>
+        <v>93.563691486098463</v>
       </c>
       <c r="F127">
         <f t="shared" ca="1" si="4"/>
-        <v>108.73707171117999</v>
+        <v>195.3962888806189</v>
       </c>
       <c r="G127">
         <f t="shared" ca="1" si="5"/>
-        <v>1586.8101978834902</v>
+        <v>4359.9992343652038</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -5413,15 +5413,15 @@
       </c>
       <c r="E128">
         <f t="shared" ca="1" si="3"/>
-        <v>92.538252321834719</v>
+        <v>40.359900807104324</v>
       </c>
       <c r="F128">
         <f t="shared" ca="1" si="4"/>
-        <v>185.26791088743335</v>
+        <v>100.93135365273295</v>
       </c>
       <c r="G128">
         <f t="shared" ca="1" si="5"/>
-        <v>7944.204590645787</v>
+        <v>4114.272306523967</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -5439,15 +5439,15 @@
       </c>
       <c r="E129">
         <f t="shared" ca="1" si="3"/>
-        <v>23.065977436427431</v>
+        <v>85.532343545946674</v>
       </c>
       <c r="F129">
         <f t="shared" ca="1" si="4"/>
-        <v>181.84368060444308</v>
+        <v>177.90390669104005</v>
       </c>
       <c r="G129">
         <f t="shared" ca="1" si="5"/>
-        <v>4856.8689412843933</v>
+        <v>8652.2310074616671</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -5465,15 +5465,15 @@
       </c>
       <c r="E130">
         <f t="shared" ca="1" si="3"/>
-        <v>84.119230870101404</v>
+        <v>77.790630190155071</v>
       </c>
       <c r="F130">
         <f t="shared" ca="1" si="4"/>
-        <v>158.07538886966387</v>
+        <v>141.23848586344252</v>
       </c>
       <c r="G130">
         <f t="shared" ca="1" si="5"/>
-        <v>797.60705118957048</v>
+        <v>3053.0627545335033</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -5491,15 +5491,15 @@
       </c>
       <c r="E131">
         <f t="shared" ref="E131:E183" ca="1" si="6">RAND()*100</f>
-        <v>72.231372962496934</v>
+        <v>48.581204024441661</v>
       </c>
       <c r="F131">
         <f t="shared" ref="F131:F183" ca="1" si="7">100+RAND()*100</f>
-        <v>106.48457179163418</v>
+        <v>140.40558803117528</v>
       </c>
       <c r="G131">
         <f t="shared" ref="G131:G183" ca="1" si="8">RAND()*10000</f>
-        <v>3679.0045294894126</v>
+        <v>634.44162638369824</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -5517,15 +5517,15 @@
       </c>
       <c r="E132">
         <f t="shared" ca="1" si="6"/>
-        <v>21.859826185055176</v>
+        <v>76.488989106353984</v>
       </c>
       <c r="F132">
         <f t="shared" ca="1" si="7"/>
-        <v>196.13726286523101</v>
+        <v>172.3715980088939</v>
       </c>
       <c r="G132">
         <f t="shared" ca="1" si="8"/>
-        <v>9656.7330246810052</v>
+        <v>9819.0405869066126</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -5543,15 +5543,15 @@
       </c>
       <c r="E133">
         <f t="shared" ca="1" si="6"/>
-        <v>90.411133008180116</v>
+        <v>67.703719763012799</v>
       </c>
       <c r="F133">
         <f t="shared" ca="1" si="7"/>
-        <v>164.93004305782756</v>
+        <v>121.41507389790426</v>
       </c>
       <c r="G133">
         <f t="shared" ca="1" si="8"/>
-        <v>4047.6345642883193</v>
+        <v>8295.9490130819358</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -5569,15 +5569,15 @@
       </c>
       <c r="E134">
         <f t="shared" ca="1" si="6"/>
-        <v>1.8100881087512732</v>
+        <v>63.321753111346737</v>
       </c>
       <c r="F134">
         <f t="shared" ca="1" si="7"/>
-        <v>182.70963894040108</v>
+        <v>111.58459711265168</v>
       </c>
       <c r="G134">
         <f t="shared" ca="1" si="8"/>
-        <v>4974.905620433824</v>
+        <v>359.24740687611643</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -5595,15 +5595,15 @@
       </c>
       <c r="E135">
         <f t="shared" ca="1" si="6"/>
-        <v>28.735883027604004</v>
+        <v>10.119104540378832</v>
       </c>
       <c r="F135">
         <f t="shared" ca="1" si="7"/>
-        <v>103.08119556259697</v>
+        <v>156.17888397910951</v>
       </c>
       <c r="G135">
         <f t="shared" ca="1" si="8"/>
-        <v>2764.5170564899613</v>
+        <v>5561.6255300840448</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -5621,15 +5621,15 @@
       </c>
       <c r="E136">
         <f t="shared" ca="1" si="6"/>
-        <v>80.061262102508195</v>
+        <v>82.378996102800784</v>
       </c>
       <c r="F136">
         <f t="shared" ca="1" si="7"/>
-        <v>126.04084302307889</v>
+        <v>193.40741647729783</v>
       </c>
       <c r="G136">
         <f t="shared" ca="1" si="8"/>
-        <v>554.95896722008274</v>
+        <v>1505.4800468758733</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -5647,15 +5647,15 @@
       </c>
       <c r="E137">
         <f t="shared" ca="1" si="6"/>
-        <v>32.013222093430706</v>
+        <v>92.174162856012614</v>
       </c>
       <c r="F137">
         <f t="shared" ca="1" si="7"/>
-        <v>191.54470232215218</v>
+        <v>168.15643449819407</v>
       </c>
       <c r="G137">
         <f t="shared" ca="1" si="8"/>
-        <v>8826.4899339212589</v>
+        <v>7851.0547869169959</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -5673,15 +5673,15 @@
       </c>
       <c r="E138">
         <f t="shared" ca="1" si="6"/>
-        <v>42.161007133342821</v>
+        <v>47.082585477625649</v>
       </c>
       <c r="F138">
         <f t="shared" ca="1" si="7"/>
-        <v>122.44553240524556</v>
+        <v>161.54402171161908</v>
       </c>
       <c r="G138">
         <f t="shared" ca="1" si="8"/>
-        <v>2443.1295902954353</v>
+        <v>5844.5423269571338</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -5699,15 +5699,15 @@
       </c>
       <c r="E139">
         <f t="shared" ca="1" si="6"/>
-        <v>50.205490842203503</v>
+        <v>59.325075579253493</v>
       </c>
       <c r="F139">
         <f t="shared" ca="1" si="7"/>
-        <v>194.48356028476633</v>
+        <v>102.39283541406144</v>
       </c>
       <c r="G139">
         <f t="shared" ca="1" si="8"/>
-        <v>3312.7609931349002</v>
+        <v>8643.1348563525917</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -5725,15 +5725,15 @@
       </c>
       <c r="E140">
         <f t="shared" ca="1" si="6"/>
-        <v>42.561261770119209</v>
+        <v>22.772303266691416</v>
       </c>
       <c r="F140">
         <f t="shared" ca="1" si="7"/>
-        <v>196.81652610269452</v>
+        <v>184.71808456411725</v>
       </c>
       <c r="G140">
         <f t="shared" ca="1" si="8"/>
-        <v>7792.5673051519052</v>
+        <v>1876.8759198337625</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -5751,15 +5751,15 @@
       </c>
       <c r="E141">
         <f t="shared" ca="1" si="6"/>
-        <v>1.1707480588071029</v>
+        <v>6.5168429596616058</v>
       </c>
       <c r="F141">
         <f t="shared" ca="1" si="7"/>
-        <v>125.46164372054832</v>
+        <v>144.53321504161752</v>
       </c>
       <c r="G141">
         <f t="shared" ca="1" si="8"/>
-        <v>4590.8026398389202</v>
+        <v>8511.8755065609075</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -5777,15 +5777,15 @@
       </c>
       <c r="E142">
         <f t="shared" ca="1" si="6"/>
-        <v>60.242542606960789</v>
+        <v>91.241462535091671</v>
       </c>
       <c r="F142">
         <f t="shared" ca="1" si="7"/>
-        <v>165.29856495956426</v>
+        <v>178.59740032189731</v>
       </c>
       <c r="G142">
         <f t="shared" ca="1" si="8"/>
-        <v>4460.0159278136653</v>
+        <v>3179.7617618998697</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -5803,15 +5803,15 @@
       </c>
       <c r="E143">
         <f t="shared" ca="1" si="6"/>
-        <v>13.998994526725305</v>
+        <v>38.802245520656498</v>
       </c>
       <c r="F143">
         <f t="shared" ca="1" si="7"/>
-        <v>181.23446254448288</v>
+        <v>189.07755766148404</v>
       </c>
       <c r="G143">
         <f t="shared" ca="1" si="8"/>
-        <v>2784.0498956774672</v>
+        <v>4050.9329884349299</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -5829,15 +5829,15 @@
       </c>
       <c r="E144">
         <f t="shared" ca="1" si="6"/>
-        <v>53.375487184641557</v>
+        <v>59.665108874546377</v>
       </c>
       <c r="F144">
         <f t="shared" ca="1" si="7"/>
-        <v>197.35702093964721</v>
+        <v>157.82945708018451</v>
       </c>
       <c r="G144">
         <f t="shared" ca="1" si="8"/>
-        <v>9770.3260240835989</v>
+        <v>9260.6611300616169</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -5855,15 +5855,15 @@
       </c>
       <c r="E145">
         <f t="shared" ca="1" si="6"/>
-        <v>4.7404333144585369</v>
+        <v>71.874322367777864</v>
       </c>
       <c r="F145">
         <f t="shared" ca="1" si="7"/>
-        <v>176.80444824042769</v>
+        <v>173.57847799999456</v>
       </c>
       <c r="G145">
         <f t="shared" ca="1" si="8"/>
-        <v>2966.2865562201914</v>
+        <v>3906.7409685154098</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -5881,15 +5881,15 @@
       </c>
       <c r="E146">
         <f t="shared" ca="1" si="6"/>
-        <v>90.299270791770894</v>
+        <v>19.61729755260999</v>
       </c>
       <c r="F146">
         <f t="shared" ca="1" si="7"/>
-        <v>100.67559516963929</v>
+        <v>157.96841642741578</v>
       </c>
       <c r="G146">
         <f t="shared" ca="1" si="8"/>
-        <v>6249.5394448015295</v>
+        <v>5246.8166419569252</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -5907,15 +5907,15 @@
       </c>
       <c r="E147">
         <f t="shared" ca="1" si="6"/>
-        <v>63.406225287155614</v>
+        <v>79.10781556293081</v>
       </c>
       <c r="F147">
         <f t="shared" ca="1" si="7"/>
-        <v>107.89001274277229</v>
+        <v>134.77987973554099</v>
       </c>
       <c r="G147">
         <f t="shared" ca="1" si="8"/>
-        <v>6729.1604536584618</v>
+        <v>2648.0620340989503</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -5933,15 +5933,15 @@
       </c>
       <c r="E148">
         <f t="shared" ca="1" si="6"/>
-        <v>22.957220105470199</v>
+        <v>56.215726636489315</v>
       </c>
       <c r="F148">
         <f t="shared" ca="1" si="7"/>
-        <v>193.97491628783473</v>
+        <v>182.94931072531688</v>
       </c>
       <c r="G148">
         <f t="shared" ca="1" si="8"/>
-        <v>2124.649497929604</v>
+        <v>6106.2474203622478</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -5959,15 +5959,15 @@
       </c>
       <c r="E149">
         <f t="shared" ca="1" si="6"/>
-        <v>26.933941979904098</v>
+        <v>83.876183371456079</v>
       </c>
       <c r="F149">
         <f t="shared" ca="1" si="7"/>
-        <v>175.48293334470429</v>
+        <v>177.15446318903312</v>
       </c>
       <c r="G149">
         <f t="shared" ca="1" si="8"/>
-        <v>6741.7917585939458</v>
+        <v>4526.8385998132635</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5985,15 +5985,15 @@
       </c>
       <c r="E150">
         <f t="shared" ca="1" si="6"/>
-        <v>55.251252507073964</v>
+        <v>11.296382865997213</v>
       </c>
       <c r="F150">
         <f t="shared" ca="1" si="7"/>
-        <v>188.14416025976215</v>
+        <v>107.20587102100504</v>
       </c>
       <c r="G150">
         <f t="shared" ca="1" si="8"/>
-        <v>249.71747563390934</v>
+        <v>3068.5344143460379</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -6011,15 +6011,15 @@
       </c>
       <c r="E151">
         <f t="shared" ca="1" si="6"/>
-        <v>11.629151518404646</v>
+        <v>71.428444132252949</v>
       </c>
       <c r="F151">
         <f t="shared" ca="1" si="7"/>
-        <v>100.61769663240233</v>
+        <v>102.77418224687277</v>
       </c>
       <c r="G151">
         <f t="shared" ca="1" si="8"/>
-        <v>2134.2769653697046</v>
+        <v>2169.6962749284885</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -6037,15 +6037,15 @@
       </c>
       <c r="E152">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4609762295003677</v>
+        <v>50.264662232998191</v>
       </c>
       <c r="F152">
         <f t="shared" ca="1" si="7"/>
-        <v>100.60288298450511</v>
+        <v>125.59932298979598</v>
       </c>
       <c r="G152">
         <f t="shared" ca="1" si="8"/>
-        <v>8971.9597371687323</v>
+        <v>7897.1989426560585</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -6063,15 +6063,15 @@
       </c>
       <c r="E153">
         <f t="shared" ca="1" si="6"/>
-        <v>32.666617935193145</v>
+        <v>91.533236599983795</v>
       </c>
       <c r="F153">
         <f t="shared" ca="1" si="7"/>
-        <v>175.80749870509493</v>
+        <v>153.94764903912298</v>
       </c>
       <c r="G153">
         <f t="shared" ca="1" si="8"/>
-        <v>2740.3634643492869</v>
+        <v>8234.2907228202348</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -6089,15 +6089,15 @@
       </c>
       <c r="E154">
         <f t="shared" ca="1" si="6"/>
-        <v>7.5488370800769422</v>
+        <v>28.365639933454535</v>
       </c>
       <c r="F154">
         <f t="shared" ca="1" si="7"/>
-        <v>152.41515093672635</v>
+        <v>142.88152430217866</v>
       </c>
       <c r="G154">
         <f t="shared" ca="1" si="8"/>
-        <v>4233.0190488557537</v>
+        <v>2663.0420439229351</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -6115,15 +6115,15 @@
       </c>
       <c r="E155">
         <f t="shared" ca="1" si="6"/>
-        <v>12.053286763765247</v>
+        <v>32.299354845409866</v>
       </c>
       <c r="F155">
         <f t="shared" ca="1" si="7"/>
-        <v>182.15549940543877</v>
+        <v>147.47562971128838</v>
       </c>
       <c r="G155">
         <f t="shared" ca="1" si="8"/>
-        <v>6409.0522192453191</v>
+        <v>4719.9942389712605</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -6141,15 +6141,15 @@
       </c>
       <c r="E156">
         <f t="shared" ca="1" si="6"/>
-        <v>50.821173412407184</v>
+        <v>83.901739861565332</v>
       </c>
       <c r="F156">
         <f t="shared" ca="1" si="7"/>
-        <v>189.69833985934335</v>
+        <v>154.97239692118242</v>
       </c>
       <c r="G156">
         <f t="shared" ca="1" si="8"/>
-        <v>6328.2990243995173</v>
+        <v>174.92893537446764</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -6167,15 +6167,15 @@
       </c>
       <c r="E157">
         <f t="shared" ca="1" si="6"/>
-        <v>18.179182204374335</v>
+        <v>53.775112859992468</v>
       </c>
       <c r="F157">
         <f t="shared" ca="1" si="7"/>
-        <v>197.07447627429138</v>
+        <v>124.663736843191</v>
       </c>
       <c r="G157">
         <f t="shared" ca="1" si="8"/>
-        <v>8993.8875488417489</v>
+        <v>7313.1171808870567</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -6193,15 +6193,15 @@
       </c>
       <c r="E158">
         <f t="shared" ca="1" si="6"/>
-        <v>65.395552561084486</v>
+        <v>10.795714468778995</v>
       </c>
       <c r="F158">
         <f t="shared" ca="1" si="7"/>
-        <v>177.1154509519188</v>
+        <v>100.31995691523929</v>
       </c>
       <c r="G158">
         <f t="shared" ca="1" si="8"/>
-        <v>2053.2627823855432</v>
+        <v>6851.9749506840326</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -6219,15 +6219,15 @@
       </c>
       <c r="E159">
         <f t="shared" ca="1" si="6"/>
-        <v>1.569529122517388</v>
+        <v>46.169219316727315</v>
       </c>
       <c r="F159">
         <f t="shared" ca="1" si="7"/>
-        <v>190.07293344392025</v>
+        <v>103.70025816544586</v>
       </c>
       <c r="G159">
         <f t="shared" ca="1" si="8"/>
-        <v>1950.8424936826696</v>
+        <v>2444.3693658469956</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -6245,15 +6245,15 @@
       </c>
       <c r="E160">
         <f t="shared" ca="1" si="6"/>
-        <v>79.491754801772245</v>
+        <v>79.331346196115575</v>
       </c>
       <c r="F160">
         <f t="shared" ca="1" si="7"/>
-        <v>117.42653580615007</v>
+        <v>199.11542113155656</v>
       </c>
       <c r="G160">
         <f t="shared" ca="1" si="8"/>
-        <v>4395.6443315651341</v>
+        <v>9294.9573634555491</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -6271,15 +6271,15 @@
       </c>
       <c r="E161">
         <f t="shared" ca="1" si="6"/>
-        <v>5.6732848886997145</v>
+        <v>7.7244938194887203</v>
       </c>
       <c r="F161">
         <f t="shared" ca="1" si="7"/>
-        <v>198.03357270537273</v>
+        <v>162.24861806031123</v>
       </c>
       <c r="G161">
         <f t="shared" ca="1" si="8"/>
-        <v>7510.2288055626886</v>
+        <v>4544.1096170776655</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -6297,15 +6297,15 @@
       </c>
       <c r="E162">
         <f t="shared" ca="1" si="6"/>
-        <v>26.00286260155319</v>
+        <v>89.237934201085267</v>
       </c>
       <c r="F162">
         <f t="shared" ca="1" si="7"/>
-        <v>111.71886864311649</v>
+        <v>100.33101738774776</v>
       </c>
       <c r="G162">
         <f t="shared" ca="1" si="8"/>
-        <v>635.91289953039313</v>
+        <v>1097.7277767321548</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -6323,15 +6323,15 @@
       </c>
       <c r="E163">
         <f t="shared" ca="1" si="6"/>
-        <v>18.132715046380866</v>
+        <v>97.635662630309156</v>
       </c>
       <c r="F163">
         <f t="shared" ca="1" si="7"/>
-        <v>154.40532747242986</v>
+        <v>143.68476492590105</v>
       </c>
       <c r="G163">
         <f t="shared" ca="1" si="8"/>
-        <v>2383.344931764284</v>
+        <v>9775.7984272256817</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -6349,15 +6349,15 @@
       </c>
       <c r="E164">
         <f t="shared" ca="1" si="6"/>
-        <v>43.172230029305247</v>
+        <v>39.735386077072988</v>
       </c>
       <c r="F164">
         <f t="shared" ca="1" si="7"/>
-        <v>114.03017404806556</v>
+        <v>116.61302508763748</v>
       </c>
       <c r="G164">
         <f t="shared" ca="1" si="8"/>
-        <v>1136.1985074198587</v>
+        <v>5606.6821895608255</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -6375,15 +6375,15 @@
       </c>
       <c r="E165">
         <f t="shared" ca="1" si="6"/>
-        <v>77.289597068645577</v>
+        <v>63.712129889865132</v>
       </c>
       <c r="F165">
         <f t="shared" ca="1" si="7"/>
-        <v>192.65678980508849</v>
+        <v>100.11183724127314</v>
       </c>
       <c r="G165">
         <f t="shared" ca="1" si="8"/>
-        <v>2981.0093867186824</v>
+        <v>3380.4014487239888</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -6401,15 +6401,15 @@
       </c>
       <c r="E166">
         <f t="shared" ca="1" si="6"/>
-        <v>17.800861613379769</v>
+        <v>83.150686526591926</v>
       </c>
       <c r="F166">
         <f t="shared" ca="1" si="7"/>
-        <v>108.00171911143616</v>
+        <v>108.89233673599244</v>
       </c>
       <c r="G166">
         <f t="shared" ca="1" si="8"/>
-        <v>1310.6259611492655</v>
+        <v>1422.7385197808685</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -6427,15 +6427,15 @@
       </c>
       <c r="E167">
         <f t="shared" ca="1" si="6"/>
-        <v>35.474615985483574</v>
+        <v>5.4936019124816493</v>
       </c>
       <c r="F167">
         <f t="shared" ca="1" si="7"/>
-        <v>132.65279287552909</v>
+        <v>178.05173852730269</v>
       </c>
       <c r="G167">
         <f t="shared" ca="1" si="8"/>
-        <v>3581.8739408571532</v>
+        <v>5713.4313488737034</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -6453,15 +6453,15 @@
       </c>
       <c r="E168">
         <f t="shared" ca="1" si="6"/>
-        <v>46.094283218153208</v>
+        <v>38.629796174599761</v>
       </c>
       <c r="F168">
         <f t="shared" ca="1" si="7"/>
-        <v>194.7984515162251</v>
+        <v>137.41965772120017</v>
       </c>
       <c r="G168">
         <f t="shared" ca="1" si="8"/>
-        <v>7620.3210146760493</v>
+        <v>9371.7199922610835</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -6479,15 +6479,15 @@
       </c>
       <c r="E169">
         <f t="shared" ca="1" si="6"/>
-        <v>97.430451091568557</v>
+        <v>50.926995406272837</v>
       </c>
       <c r="F169">
         <f t="shared" ca="1" si="7"/>
-        <v>164.17968407549995</v>
+        <v>195.92136215141323</v>
       </c>
       <c r="G169">
         <f t="shared" ca="1" si="8"/>
-        <v>9374.3677124701389</v>
+        <v>161.56699465710855</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -6505,15 +6505,15 @@
       </c>
       <c r="E170">
         <f t="shared" ca="1" si="6"/>
-        <v>63.498083213509901</v>
+        <v>20.976237184723956</v>
       </c>
       <c r="F170">
         <f t="shared" ca="1" si="7"/>
-        <v>133.86035061681824</v>
+        <v>102.89739293599777</v>
       </c>
       <c r="G170">
         <f t="shared" ca="1" si="8"/>
-        <v>9542.0400683534062</v>
+        <v>7093.7932103497851</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -6531,15 +6531,15 @@
       </c>
       <c r="E171">
         <f t="shared" ca="1" si="6"/>
-        <v>93.218241926349663</v>
+        <v>24.372658707561754</v>
       </c>
       <c r="F171">
         <f t="shared" ca="1" si="7"/>
-        <v>112.69087819047631</v>
+        <v>164.32422519469134</v>
       </c>
       <c r="G171">
         <f t="shared" ca="1" si="8"/>
-        <v>1377.5214198048814</v>
+        <v>3277.019023027995</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -6557,15 +6557,15 @@
       </c>
       <c r="E172">
         <f t="shared" ca="1" si="6"/>
-        <v>47.221770740747239</v>
+        <v>66.104894077940884</v>
       </c>
       <c r="F172">
         <f t="shared" ca="1" si="7"/>
-        <v>118.07603437112135</v>
+        <v>196.52449849679007</v>
       </c>
       <c r="G172">
         <f t="shared" ca="1" si="8"/>
-        <v>6235.6263356135714</v>
+        <v>9291.1264938834265</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -6583,15 +6583,15 @@
       </c>
       <c r="E173">
         <f t="shared" ca="1" si="6"/>
-        <v>34.209035163145941</v>
+        <v>14.264850125655926</v>
       </c>
       <c r="F173">
         <f t="shared" ca="1" si="7"/>
-        <v>134.32015025204342</v>
+        <v>118.05192827709264</v>
       </c>
       <c r="G173">
         <f t="shared" ca="1" si="8"/>
-        <v>7181.0906315975253</v>
+        <v>432.56339706174043</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -6609,15 +6609,15 @@
       </c>
       <c r="E174">
         <f t="shared" ca="1" si="6"/>
-        <v>61.094377021063472</v>
+        <v>71.904047176551231</v>
       </c>
       <c r="F174">
         <f t="shared" ca="1" si="7"/>
-        <v>138.49126583902807</v>
+        <v>137.55380814705748</v>
       </c>
       <c r="G174">
         <f t="shared" ca="1" si="8"/>
-        <v>7077.2382433874118</v>
+        <v>780.64701942967997</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -6635,15 +6635,15 @@
       </c>
       <c r="E175">
         <f t="shared" ca="1" si="6"/>
-        <v>19.801715424798982</v>
+        <v>63.621612634995472</v>
       </c>
       <c r="F175">
         <f t="shared" ca="1" si="7"/>
-        <v>116.77625958943098</v>
+        <v>115.08667969947112</v>
       </c>
       <c r="G175">
         <f t="shared" ca="1" si="8"/>
-        <v>9740.3114487537296</v>
+        <v>7376.7843191665816</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -6661,15 +6661,15 @@
       </c>
       <c r="E176">
         <f t="shared" ca="1" si="6"/>
-        <v>28.098190344357722</v>
+        <v>20.279280084613106</v>
       </c>
       <c r="F176">
         <f t="shared" ca="1" si="7"/>
-        <v>168.62671973684178</v>
+        <v>115.57394328921286</v>
       </c>
       <c r="G176">
         <f t="shared" ca="1" si="8"/>
-        <v>2104.9070404192826</v>
+        <v>6069.8516051035958</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -6687,15 +6687,15 @@
       </c>
       <c r="E177">
         <f t="shared" ca="1" si="6"/>
-        <v>95.802732669228391</v>
+        <v>10.843823418791665</v>
       </c>
       <c r="F177">
         <f t="shared" ca="1" si="7"/>
-        <v>189.48856778213855</v>
+        <v>196.97415062177447</v>
       </c>
       <c r="G177">
         <f t="shared" ca="1" si="8"/>
-        <v>3245.0176643941022</v>
+        <v>9076.3703038402</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -6713,15 +6713,15 @@
       </c>
       <c r="E178">
         <f t="shared" ca="1" si="6"/>
-        <v>74.422683831381235</v>
+        <v>17.82637114483423</v>
       </c>
       <c r="F178">
         <f t="shared" ca="1" si="7"/>
-        <v>144.41753843551243</v>
+        <v>143.9177279669731</v>
       </c>
       <c r="G178">
         <f t="shared" ca="1" si="8"/>
-        <v>4233.8452816637919</v>
+        <v>196.42104920003399</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -6739,15 +6739,15 @@
       </c>
       <c r="E179">
         <f t="shared" ca="1" si="6"/>
-        <v>61.376142957247957</v>
+        <v>65.056269284384911</v>
       </c>
       <c r="F179">
         <f t="shared" ca="1" si="7"/>
-        <v>173.25684075535577</v>
+        <v>152.1553128203189</v>
       </c>
       <c r="G179">
         <f t="shared" ca="1" si="8"/>
-        <v>4334.3155701054866</v>
+        <v>9781.4717269323573</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -6765,15 +6765,15 @@
       </c>
       <c r="E180">
         <f t="shared" ca="1" si="6"/>
-        <v>19.513130369567612</v>
+        <v>24.933892488285856</v>
       </c>
       <c r="F180">
         <f t="shared" ca="1" si="7"/>
-        <v>106.42044156796024</v>
+        <v>102.76798477762974</v>
       </c>
       <c r="G180">
         <f t="shared" ca="1" si="8"/>
-        <v>4910.3281910860023</v>
+        <v>7351.0677686970503</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -6791,15 +6791,15 @@
       </c>
       <c r="E181">
         <f t="shared" ca="1" si="6"/>
-        <v>12.489563381317314</v>
+        <v>21.412461950005024</v>
       </c>
       <c r="F181">
         <f t="shared" ca="1" si="7"/>
-        <v>182.75270852507043</v>
+        <v>103.12551713702899</v>
       </c>
       <c r="G181">
         <f t="shared" ca="1" si="8"/>
-        <v>1691.1192378216622</v>
+        <v>6670.7613208206631</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -6817,15 +6817,15 @@
       </c>
       <c r="E182">
         <f t="shared" ca="1" si="6"/>
-        <v>23.927037698124099</v>
+        <v>93.071404725099526</v>
       </c>
       <c r="F182">
         <f t="shared" ca="1" si="7"/>
-        <v>115.549134553</v>
+        <v>125.98505235856985</v>
       </c>
       <c r="G182">
         <f t="shared" ca="1" si="8"/>
-        <v>7316.8431892875251</v>
+        <v>1945.9291915342535</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -6843,15 +6843,15 @@
       </c>
       <c r="E183">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7437349090103869</v>
+        <v>30.171027417006002</v>
       </c>
       <c r="F183">
         <f t="shared" ca="1" si="7"/>
-        <v>100.20748074739664</v>
+        <v>111.49821870240993</v>
       </c>
       <c r="G183">
         <f t="shared" ca="1" si="8"/>
-        <v>1450.6768812729276</v>
+        <v>268.90169032230295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>